<commit_message>
Some corrections due to package upgrades
</commit_message>
<xml_diff>
--- a/tests/data/unittest_testset_aanvullende_regels.xlsx
+++ b/tests/data/unittest_testset_aanvullende_regels.xlsx
@@ -1,24 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan_h_000\Documents\DNB\Python\solvency2-rules\tests\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5712F9C-D0D0-418B-95D0-EF84C91D9E96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="18000" windowHeight="9360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="18000" windowHeight="9360"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$H$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$H$9</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -160,8 +154,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,9 +225,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -271,9 +265,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -305,27 +299,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -357,27 +333,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -550,14 +508,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:E2"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
@@ -569,7 +527,7 @@
     <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="3" t="s">
         <v>33</v>
       </c>
@@ -598,7 +556,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -624,7 +582,7 @@
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="1" customFormat="1">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -650,7 +608,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" s="1" customFormat="1">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -676,7 +634,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="1" customFormat="1">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -702,7 +660,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="1" customFormat="1">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -728,7 +686,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="1" customFormat="1">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -751,7 +709,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="1" customFormat="1">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -774,7 +732,6 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>